<commit_message>
Localizing the Github Repo
Adding/Removing/Localizing files in the repo so we can start modifying the source code as a team.
</commit_message>
<xml_diff>
--- a/Scheduling/Schedule/Schedule-Team4.xlsx
+++ b/Scheduling/Schedule/Schedule-Team4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\School Account\Desktop\Team4Project\Scheduling\Schedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7BFD9DE0-C796-4CFD-82EF-70BDDF744D9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D97E701-5807-41B8-A5E3-CBE4D0F55F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="1" r:id="rId1"/>
@@ -97,15 +97,6 @@
     <t>002a</t>
   </si>
   <si>
-    <t>Chase updating Team Schedule</t>
-  </si>
-  <si>
-    <t>Team Members updating schedule</t>
-  </si>
-  <si>
-    <t>Populate Jira roadmap</t>
-  </si>
-  <si>
     <t>Set up Chase with Jira</t>
   </si>
   <si>
@@ -133,18 +124,6 @@
     <t>004a</t>
   </si>
   <si>
-    <t>Chase's GitHub created and linked</t>
-  </si>
-  <si>
-    <t>Austin's GitHub created and linked</t>
-  </si>
-  <si>
-    <t>Cade's GitHub created and linked</t>
-  </si>
-  <si>
-    <t>Cole's GitHub created and linked</t>
-  </si>
-  <si>
     <t>004b</t>
   </si>
   <si>
@@ -157,18 +136,9 @@
     <t>004e</t>
   </si>
   <si>
-    <t>Chase's VM Running</t>
-  </si>
-  <si>
     <t>Austin's VM Running</t>
   </si>
   <si>
-    <t>Cade's VM Running</t>
-  </si>
-  <si>
-    <t>Cole's VM Running</t>
-  </si>
-  <si>
     <t>005a</t>
   </si>
   <si>
@@ -193,45 +163,6 @@
     <t>Cole</t>
   </si>
   <si>
-    <t>Chase's Installation is running</t>
-  </si>
-  <si>
-    <t>Github Repository created</t>
-  </si>
-  <si>
-    <t>Austin's Installation is running</t>
-  </si>
-  <si>
-    <t>Cade's Installation is running</t>
-  </si>
-  <si>
-    <t>Cole's Installation is running</t>
-  </si>
-  <si>
-    <t>MRI Tech Persona</t>
-  </si>
-  <si>
-    <t>Ultrasound Tech Persona</t>
-  </si>
-  <si>
-    <t>Front Desk Worker Persona</t>
-  </si>
-  <si>
-    <t>Guest Persona</t>
-  </si>
-  <si>
-    <t>Physician Persona</t>
-  </si>
-  <si>
-    <t>IT Department Persona</t>
-  </si>
-  <si>
-    <t>Radiologist Persona</t>
-  </si>
-  <si>
-    <t>Student Persona</t>
-  </si>
-  <si>
     <t>006a</t>
   </si>
   <si>
@@ -457,9 +388,6 @@
     <t>IT Department.txt</t>
   </si>
   <si>
-    <t>Student.txt</t>
-  </si>
-  <si>
     <t>Ideas of Features</t>
   </si>
   <si>
@@ -599,6 +527,78 @@
   </si>
   <si>
     <t>Database Requirments learned</t>
+  </si>
+  <si>
+    <t>Populate the Jira roadmap</t>
+  </si>
+  <si>
+    <t>Get Cole's VM Running</t>
+  </si>
+  <si>
+    <t>Get Cade's VM Running</t>
+  </si>
+  <si>
+    <t>Get Chase's VM Running</t>
+  </si>
+  <si>
+    <t>Get Chase's Installation is running</t>
+  </si>
+  <si>
+    <t>Get Austin's Installation is running</t>
+  </si>
+  <si>
+    <t>Get Cade's Installation is running</t>
+  </si>
+  <si>
+    <t>Get Cole's Installation is running</t>
+  </si>
+  <si>
+    <t>Create MRI Tech Persona</t>
+  </si>
+  <si>
+    <t>Create Ultrasound Tech Persona</t>
+  </si>
+  <si>
+    <t>Create Front Desk Worker Persona</t>
+  </si>
+  <si>
+    <t>Create Guest Persona</t>
+  </si>
+  <si>
+    <t>Create Physician Persona</t>
+  </si>
+  <si>
+    <t>Create IT Department Persona</t>
+  </si>
+  <si>
+    <t>Create Radiologist Persona</t>
+  </si>
+  <si>
+    <t>Create Transporter Persona</t>
+  </si>
+  <si>
+    <t>Transporter.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create and install Chase's GitHub </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create and install Austin's GitHub </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create and install Cade's GitHub </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create and install Cole's GitHub </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Have team members update schedule </t>
+  </si>
+  <si>
+    <t>Maintaining the System Schedule</t>
+  </si>
+  <si>
+    <t>Create Team Github Repository</t>
   </si>
 </sst>
 </file>
@@ -1145,10 +1145,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>61.55</c:v>
+                  <c:v>66.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>80</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3126,8 +3126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M49" sqref="M49"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3212,15 +3212,15 @@
       </c>
       <c r="H2" s="10">
         <f>SUM(H3:H100)</f>
-        <v>141.55000000000001</v>
+        <v>182.5</v>
       </c>
       <c r="I2" s="14">
         <f>SUM(I3:I100)</f>
-        <v>61.55</v>
+        <v>66.5</v>
       </c>
       <c r="J2" s="14">
         <f>SUM(J3:J100)</f>
-        <v>80</v>
+        <v>116</v>
       </c>
       <c r="K2" s="17"/>
       <c r="L2" s="17"/>
@@ -3258,7 +3258,7 @@
         <v>19</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>20</v>
+        <v>186</v>
       </c>
       <c r="C4" s="3">
         <v>44596</v>
@@ -3283,13 +3283,13 @@
         <v>2</v>
       </c>
       <c r="K4" s="19" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="L4" s="19" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="M4" s="19" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="N4" s="11" t="str">
         <f t="shared" ref="N4:N67" si="1">IF(A4="","",IF(I4="","Not Started",IF(H4=I4,"Complete",IF(H4&gt;I4,"In Progress"))))</f>
@@ -3298,10 +3298,10 @@
     </row>
     <row r="5" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>21</v>
+        <v>185</v>
       </c>
       <c r="C5" s="3">
         <v>44596</v>
@@ -3326,13 +3326,13 @@
         <v>2.5</v>
       </c>
       <c r="K5" s="19" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="L5" s="19" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="M5" s="19" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="N5" s="11" t="str">
         <f t="shared" si="1"/>
@@ -3344,7 +3344,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>164</v>
       </c>
       <c r="C6" s="3">
         <v>44599</v>
@@ -3369,13 +3369,13 @@
         <v>1.5</v>
       </c>
       <c r="K6" s="19" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="L6" s="19" t="s">
-        <v>126</v>
+        <v>103</v>
       </c>
       <c r="M6" s="19" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="N6" s="11" t="str">
         <f>IF(A6="","",IF(I6="","Not Started",IF(H6=I6,"Complete",IF(H6&gt;I6,"In Progress"))))</f>
@@ -3387,7 +3387,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C7" s="3">
         <v>44599</v>
@@ -3402,23 +3402,23 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="H7" s="4">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="I7" s="4">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="J7" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K7" s="19" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="L7" s="19" t="s">
-        <v>160</v>
+        <v>136</v>
       </c>
       <c r="M7" s="19" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="N7" s="11" t="str">
         <f t="shared" si="1"/>
@@ -3427,10 +3427,10 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C8" s="3">
         <v>44599</v>
@@ -3445,23 +3445,23 @@
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="4">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="I8" s="4">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="J8" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K8" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="L8" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="L8" s="19" t="s">
-        <v>152</v>
-      </c>
       <c r="M8" s="19" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="N8" s="11" t="str">
         <f t="shared" si="1"/>
@@ -3470,10 +3470,10 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C9" s="3">
         <v>44599</v>
@@ -3488,23 +3488,23 @@
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="4">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="I9" s="4">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="J9" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K9" s="19" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="L9" s="19" t="s">
-        <v>153</v>
+        <v>129</v>
       </c>
       <c r="M9" s="19" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="N9" s="11" t="str">
         <f t="shared" si="1"/>
@@ -3513,10 +3513,10 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C10" s="3">
         <v>44599</v>
@@ -3531,23 +3531,23 @@
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="4">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="I10" s="4">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="J10" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K10" s="19" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="L10" s="19" t="s">
-        <v>154</v>
+        <v>130</v>
       </c>
       <c r="M10" s="19" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="N10" s="11" t="str">
         <f t="shared" si="1"/>
@@ -3556,10 +3556,10 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>53</v>
+        <v>187</v>
       </c>
       <c r="C11" s="22">
         <v>44606</v>
@@ -3574,23 +3574,23 @@
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="4">
-        <v>0.75</v>
+        <v>2</v>
       </c>
       <c r="I11" s="4">
-        <v>0.75</v>
+        <v>2</v>
       </c>
       <c r="J11" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K11" s="20" t="s">
-        <v>129</v>
+        <v>106</v>
       </c>
       <c r="L11" s="19" t="s">
-        <v>159</v>
+        <v>135</v>
       </c>
       <c r="M11" s="19" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="N11" s="11" t="str">
         <f t="shared" si="1"/>
@@ -3599,10 +3599,10 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>32</v>
+        <v>181</v>
       </c>
       <c r="C12" s="22">
         <v>44606</v>
@@ -3617,23 +3617,23 @@
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="4">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="I12" s="4">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="J12" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K12" s="19" t="s">
-        <v>129</v>
+        <v>106</v>
       </c>
       <c r="L12" s="19" t="s">
-        <v>155</v>
+        <v>131</v>
       </c>
       <c r="M12" s="19" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="N12" s="11" t="str">
         <f t="shared" si="1"/>
@@ -3642,10 +3642,10 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>33</v>
+        <v>182</v>
       </c>
       <c r="C13" s="22">
         <v>44606</v>
@@ -3660,23 +3660,23 @@
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
       <c r="H13" s="4">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="I13" s="4">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="J13" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K13" s="19" t="s">
-        <v>129</v>
+        <v>106</v>
       </c>
       <c r="L13" s="19" t="s">
-        <v>156</v>
+        <v>132</v>
       </c>
       <c r="M13" s="19" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="N13" s="11" t="str">
         <f t="shared" si="1"/>
@@ -3685,10 +3685,10 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>34</v>
+        <v>183</v>
       </c>
       <c r="C14" s="22">
         <v>44606</v>
@@ -3703,23 +3703,23 @@
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
       <c r="H14" s="4">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="I14" s="4">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="J14" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K14" s="19" t="s">
-        <v>129</v>
+        <v>106</v>
       </c>
       <c r="L14" s="19" t="s">
-        <v>157</v>
+        <v>133</v>
       </c>
       <c r="M14" s="19" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="N14" s="11" t="str">
         <f t="shared" si="1"/>
@@ -3728,10 +3728,10 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>35</v>
+        <v>184</v>
       </c>
       <c r="C15" s="22">
         <v>44606</v>
@@ -3746,23 +3746,23 @@
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
       <c r="H15" s="4">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="I15" s="4">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="J15" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K15" s="19" t="s">
-        <v>129</v>
+        <v>106</v>
       </c>
       <c r="L15" s="19" t="s">
-        <v>158</v>
+        <v>134</v>
       </c>
       <c r="M15" s="19" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="N15" s="11" t="str">
         <f t="shared" si="1"/>
@@ -3771,10 +3771,10 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C16" s="22">
         <v>44607</v>
@@ -3799,13 +3799,13 @@
         <v>0</v>
       </c>
       <c r="K16" s="19" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="L16" s="19" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="M16" s="19" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="N16" s="11" t="str">
         <f>IF(A16="","",IF(I16="","Not Started",IF(H16=I16,"Complete",IF(H16&gt;I16,"In Progress"))))</f>
@@ -3814,10 +3814,10 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>43</v>
+        <v>165</v>
       </c>
       <c r="C17" s="22">
         <v>44607</v>
@@ -3832,23 +3832,23 @@
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
       <c r="H17" s="4">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="I17" s="4">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="J17" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K17" s="19" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="L17" s="19" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="M17" s="19" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="N17" s="11" t="str">
         <f>IF(A17="","",IF(I17="","Not Started",IF(H17=I17,"Complete",IF(H17&gt;I17,"In Progress"))))</f>
@@ -3857,10 +3857,10 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>42</v>
+        <v>166</v>
       </c>
       <c r="C18" s="22">
         <v>44607</v>
@@ -3885,13 +3885,13 @@
         <v>0</v>
       </c>
       <c r="K18" s="19" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="L18" s="19" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="M18" s="19" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="N18" s="11" t="str">
         <f t="shared" si="1"/>
@@ -3900,10 +3900,10 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>40</v>
+        <v>167</v>
       </c>
       <c r="C19" s="22">
         <v>44607</v>
@@ -3918,23 +3918,23 @@
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
       <c r="H19" s="4">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="I19" s="4">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="J19" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K19" s="19" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="L19" s="19" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="M19" s="19" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="N19" s="11" t="str">
         <f t="shared" si="1"/>
@@ -3943,10 +3943,10 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>52</v>
+        <v>168</v>
       </c>
       <c r="C20" s="22">
         <v>44607</v>
@@ -3971,13 +3971,13 @@
         <v>0</v>
       </c>
       <c r="K20" s="19" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="L20" s="19" t="s">
-        <v>163</v>
+        <v>139</v>
       </c>
       <c r="M20" s="19" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="N20" s="11" t="str">
         <f t="shared" si="1"/>
@@ -3986,10 +3986,10 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>54</v>
+        <v>169</v>
       </c>
       <c r="C21" s="22">
         <v>44607</v>
@@ -4014,13 +4014,13 @@
         <v>0</v>
       </c>
       <c r="K21" s="19" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="L21" s="19" t="s">
-        <v>164</v>
+        <v>140</v>
       </c>
       <c r="M21" s="19" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="N21" s="11" t="str">
         <f t="shared" si="1"/>
@@ -4029,10 +4029,10 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>55</v>
+        <v>170</v>
       </c>
       <c r="C22" s="22">
         <v>44607</v>
@@ -4047,23 +4047,23 @@
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
       <c r="H22" s="4">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="I22" s="4">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="J22" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K22" s="19" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="L22" s="19" t="s">
-        <v>165</v>
+        <v>141</v>
       </c>
       <c r="M22" s="19" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="N22" s="11" t="str">
         <f t="shared" si="1"/>
@@ -4072,10 +4072,10 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>56</v>
+        <v>171</v>
       </c>
       <c r="C23" s="22">
         <v>44607</v>
@@ -4100,13 +4100,13 @@
         <v>0</v>
       </c>
       <c r="K23" s="19" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="L23" s="19" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
       <c r="M23" s="19" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="N23" s="11" t="str">
         <f t="shared" si="1"/>
@@ -4115,10 +4115,10 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>57</v>
+        <v>172</v>
       </c>
       <c r="C24" s="22">
         <v>44604</v>
@@ -4143,13 +4143,13 @@
         <v>0</v>
       </c>
       <c r="K24" s="19" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
       <c r="L24" s="19" t="s">
-        <v>134</v>
+        <v>111</v>
       </c>
       <c r="M24" s="19" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="N24" s="11" t="str">
         <f t="shared" si="1"/>
@@ -4158,10 +4158,10 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>58</v>
+        <v>173</v>
       </c>
       <c r="C25" s="22">
         <v>44604</v>
@@ -4186,13 +4186,13 @@
         <v>0</v>
       </c>
       <c r="K25" s="19" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
       <c r="L25" s="19" t="s">
-        <v>135</v>
+        <v>112</v>
       </c>
       <c r="M25" s="19" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="N25" s="11" t="str">
         <f t="shared" si="1"/>
@@ -4201,10 +4201,10 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>59</v>
+        <v>174</v>
       </c>
       <c r="C26" s="22">
         <v>44604</v>
@@ -4229,13 +4229,13 @@
         <v>0</v>
       </c>
       <c r="K26" s="19" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="L26" s="19" t="s">
-        <v>136</v>
+        <v>113</v>
       </c>
       <c r="M26" s="19" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="N26" s="11" t="str">
         <f>IF(A26="","",IF(I26="","Not Started",IF(H26=I26,"Complete",IF(H26&gt;I26,"In Progress"))))</f>
@@ -4244,10 +4244,10 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>60</v>
+        <v>175</v>
       </c>
       <c r="C27" s="22">
         <v>44604</v>
@@ -4272,13 +4272,13 @@
         <v>0</v>
       </c>
       <c r="K27" s="19" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="L27" s="19" t="s">
-        <v>137</v>
+        <v>114</v>
       </c>
       <c r="M27" s="19" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="N27" s="11" t="str">
         <f t="shared" si="1"/>
@@ -4287,10 +4287,10 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>61</v>
+        <v>176</v>
       </c>
       <c r="C28" s="22">
         <v>44604</v>
@@ -4315,13 +4315,13 @@
         <v>0</v>
       </c>
       <c r="K28" s="19" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="L28" s="19" t="s">
-        <v>138</v>
+        <v>115</v>
       </c>
       <c r="M28" s="19" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="N28" s="11" t="str">
         <f>IF(A28="","",IF(I28="","Not Started",IF(H28=I28,"Complete",IF(H28&gt;I28,"In Progress"))))</f>
@@ -4330,10 +4330,10 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>62</v>
+        <v>177</v>
       </c>
       <c r="C29" s="22">
         <v>44604</v>
@@ -4358,13 +4358,13 @@
         <v>0</v>
       </c>
       <c r="K29" s="19" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="L29" s="19" t="s">
-        <v>139</v>
+        <v>116</v>
       </c>
       <c r="M29" s="19" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="N29" s="11" t="str">
         <f t="shared" si="1"/>
@@ -4373,10 +4373,10 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>63</v>
+        <v>178</v>
       </c>
       <c r="C30" s="22">
         <v>44604</v>
@@ -4391,23 +4391,23 @@
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
       <c r="H30" s="4">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="I30" s="4">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="J30" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K30" s="19" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="L30" s="19" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="M30" s="19" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="N30" s="11" t="str">
         <f t="shared" si="1"/>
@@ -4416,10 +4416,10 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>64</v>
+        <v>179</v>
       </c>
       <c r="C31" s="22">
         <v>44604</v>
@@ -4444,13 +4444,13 @@
         <v>0</v>
       </c>
       <c r="K31" s="19" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="L31" s="19" t="s">
-        <v>140</v>
+        <v>180</v>
       </c>
       <c r="M31" s="19" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="N31" s="11" t="str">
         <f t="shared" si="1"/>
@@ -4459,10 +4459,10 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="C32" s="22">
         <v>44604</v>
@@ -4487,13 +4487,13 @@
         <v>0</v>
       </c>
       <c r="K32" s="19" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
       <c r="L32" s="19" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="M32" s="19" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="N32" s="11" t="str">
         <f t="shared" si="1"/>
@@ -4502,10 +4502,10 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="C33" s="22">
         <v>44604</v>
@@ -4530,13 +4530,13 @@
         <v>0</v>
       </c>
       <c r="K33" s="19" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
       <c r="L33" s="19" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="M33" s="19" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="N33" s="11" t="str">
         <f t="shared" si="1"/>
@@ -4545,10 +4545,10 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="C34" s="22">
         <v>44604</v>
@@ -4573,13 +4573,13 @@
         <v>0</v>
       </c>
       <c r="K34" s="19" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
       <c r="L34" s="19" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="M34" s="19" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="N34" s="11" t="str">
         <f t="shared" si="1"/>
@@ -4588,10 +4588,10 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="C35" s="22">
         <v>44604</v>
@@ -4616,13 +4616,13 @@
         <v>0</v>
       </c>
       <c r="K35" s="19" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
       <c r="L35" s="19" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="M35" s="19" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="N35" s="11" t="str">
         <f t="shared" si="1"/>
@@ -4631,10 +4631,10 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
       <c r="C36" s="22">
         <v>44611</v>
@@ -4659,13 +4659,13 @@
         <v>2</v>
       </c>
       <c r="K36" s="19" t="s">
-        <v>142</v>
+        <v>118</v>
       </c>
       <c r="L36" s="19" t="s">
-        <v>183</v>
+        <v>159</v>
       </c>
       <c r="M36" s="19" t="s">
-        <v>181</v>
+        <v>157</v>
       </c>
       <c r="N36" s="11" t="str">
         <f t="shared" si="1"/>
@@ -4674,10 +4674,10 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="C37" s="22">
         <v>44611</v>
@@ -4702,13 +4702,13 @@
         <v>3</v>
       </c>
       <c r="K37" s="19" t="s">
-        <v>143</v>
+        <v>119</v>
       </c>
       <c r="L37" s="19" t="s">
-        <v>184</v>
+        <v>160</v>
       </c>
       <c r="M37" s="19" t="s">
-        <v>181</v>
+        <v>157</v>
       </c>
       <c r="N37" s="11" t="str">
         <f t="shared" si="1"/>
@@ -4717,10 +4717,10 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="C38" s="22">
         <v>44611</v>
@@ -4745,13 +4745,13 @@
         <v>3</v>
       </c>
       <c r="K38" s="19" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
       <c r="L38" s="19" t="s">
-        <v>185</v>
+        <v>161</v>
       </c>
       <c r="M38" s="19" t="s">
-        <v>181</v>
+        <v>157</v>
       </c>
       <c r="N38" s="11" t="str">
         <f t="shared" si="1"/>
@@ -4760,10 +4760,10 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="C39" s="22">
         <v>44611</v>
@@ -4788,13 +4788,13 @@
         <v>8</v>
       </c>
       <c r="K39" s="19" t="s">
-        <v>145</v>
+        <v>121</v>
       </c>
       <c r="L39" s="19" t="s">
-        <v>186</v>
+        <v>162</v>
       </c>
       <c r="M39" s="19" t="s">
-        <v>181</v>
+        <v>157</v>
       </c>
       <c r="N39" s="11" t="str">
         <f t="shared" si="1"/>
@@ -4803,10 +4803,10 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="C40" s="22">
         <v>44611</v>
@@ -4831,13 +4831,13 @@
         <v>6</v>
       </c>
       <c r="K40" s="19" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="L40" s="19" t="s">
-        <v>187</v>
+        <v>163</v>
       </c>
       <c r="M40" s="19" t="s">
-        <v>181</v>
+        <v>157</v>
       </c>
       <c r="N40" s="11" t="str">
         <f t="shared" si="1"/>
@@ -4846,10 +4846,10 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="C41" s="22">
         <v>44621</v>
@@ -4874,13 +4874,13 @@
         <v>0</v>
       </c>
       <c r="K41" s="19" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="L41" s="19" t="s">
-        <v>173</v>
+        <v>149</v>
       </c>
       <c r="M41" s="19" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="N41" s="11" t="str">
         <f t="shared" si="1"/>
@@ -4889,10 +4889,10 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="C42" s="22">
         <v>44621</v>
@@ -4917,13 +4917,13 @@
         <v>0</v>
       </c>
       <c r="K42" s="19" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="L42" s="19" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="M42" s="19" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="N42" s="11" t="str">
         <f t="shared" si="1"/>
@@ -4932,10 +4932,10 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="C43" s="22">
         <v>44621</v>
@@ -4960,13 +4960,13 @@
         <v>0</v>
       </c>
       <c r="K43" s="19" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="L43" s="19" t="s">
-        <v>175</v>
+        <v>151</v>
       </c>
       <c r="M43" s="19" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="N43" s="11" t="str">
         <f t="shared" si="1"/>
@@ -4975,10 +4975,10 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="C44" s="22">
         <v>44621</v>
@@ -5003,13 +5003,13 @@
         <v>0</v>
       </c>
       <c r="K44" s="19" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="L44" s="19" t="s">
-        <v>176</v>
+        <v>152</v>
       </c>
       <c r="M44" s="19" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="N44" s="11" t="str">
         <f t="shared" si="1"/>
@@ -5018,10 +5018,10 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="C45" s="22">
         <v>44621</v>
@@ -5046,13 +5046,13 @@
         <v>0</v>
       </c>
       <c r="K45" s="19" t="s">
-        <v>147</v>
+        <v>123</v>
       </c>
       <c r="L45" s="19" t="s">
-        <v>177</v>
+        <v>153</v>
       </c>
       <c r="M45" s="19" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="N45" s="11" t="str">
         <f t="shared" si="1"/>
@@ -5061,10 +5061,10 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="C46" s="22">
         <v>44621</v>
@@ -5089,13 +5089,13 @@
         <v>0</v>
       </c>
       <c r="K46" s="19" t="s">
-        <v>147</v>
+        <v>123</v>
       </c>
       <c r="L46" s="19" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="M46" s="19" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="N46" s="11" t="str">
         <f t="shared" si="1"/>
@@ -5104,10 +5104,10 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="C47" s="22">
         <v>44621</v>
@@ -5132,13 +5132,13 @@
         <v>0</v>
       </c>
       <c r="K47" s="19" t="s">
-        <v>147</v>
+        <v>123</v>
       </c>
       <c r="L47" s="19" t="s">
-        <v>178</v>
+        <v>154</v>
       </c>
       <c r="M47" s="19" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="N47" s="11" t="str">
         <f t="shared" si="1"/>
@@ -5147,10 +5147,10 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="C48" s="22">
         <v>44621</v>
@@ -5175,13 +5175,13 @@
         <v>0</v>
       </c>
       <c r="K48" s="19" t="s">
-        <v>147</v>
+        <v>123</v>
       </c>
       <c r="L48" s="19" t="s">
-        <v>180</v>
+        <v>156</v>
       </c>
       <c r="M48" s="19" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="N48" s="11" t="str">
         <f t="shared" si="1"/>
@@ -5190,10 +5190,10 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="C49" s="22">
         <v>44626</v>
@@ -5218,10 +5218,10 @@
         <v>32</v>
       </c>
       <c r="K49" s="19" t="s">
-        <v>145</v>
+        <v>121</v>
       </c>
       <c r="M49" s="19" t="s">
-        <v>182</v>
+        <v>158</v>
       </c>
       <c r="N49" s="11" t="str">
         <f t="shared" si="1"/>
@@ -5230,10 +5230,10 @@
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>100</v>
+        <v>77</v>
       </c>
       <c r="C50" s="22">
         <v>44633</v>
@@ -5258,10 +5258,10 @@
         <v>12</v>
       </c>
       <c r="K50" s="19" t="s">
-        <v>148</v>
+        <v>124</v>
       </c>
       <c r="M50" s="19" t="s">
-        <v>182</v>
+        <v>158</v>
       </c>
       <c r="N50" s="11" t="str">
         <f t="shared" si="1"/>
@@ -5270,10 +5270,10 @@
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>120</v>
+        <v>97</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="C51" s="22">
         <v>44633</v>
@@ -5298,10 +5298,10 @@
         <v>8</v>
       </c>
       <c r="K51" s="19" t="s">
-        <v>148</v>
+        <v>124</v>
       </c>
       <c r="M51" s="19" t="s">
-        <v>182</v>
+        <v>158</v>
       </c>
       <c r="N51" s="11" t="str">
         <f t="shared" si="1"/>
@@ -5310,10 +5310,10 @@
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>102</v>
+        <v>79</v>
       </c>
       <c r="C52" s="22">
         <v>44641</v>
@@ -5328,32 +5328,32 @@
       <c r="F52" s="9"/>
       <c r="G52" s="9"/>
       <c r="H52" s="4">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I52" s="4">
         <v>0</v>
       </c>
       <c r="J52" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="K52" s="19" t="s">
-        <v>149</v>
+        <v>125</v>
       </c>
       <c r="M52" s="19" t="s">
-        <v>182</v>
+        <v>158</v>
       </c>
       <c r="N52" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>Complete</v>
+        <v>In Progress</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>103</v>
+        <v>80</v>
       </c>
       <c r="C53" s="22">
         <v>44641</v>
@@ -5368,32 +5368,32 @@
       <c r="F53" s="9"/>
       <c r="G53" s="9"/>
       <c r="H53" s="4">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I53" s="4">
         <v>0</v>
       </c>
       <c r="J53" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="K53" s="19" t="s">
-        <v>150</v>
+        <v>126</v>
       </c>
       <c r="M53" s="19" t="s">
-        <v>182</v>
+        <v>158</v>
       </c>
       <c r="N53" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>Complete</v>
+        <v>In Progress</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="C54" s="22">
         <v>44641</v>
@@ -5408,24 +5408,24 @@
       <c r="F54" s="9"/>
       <c r="G54" s="9"/>
       <c r="H54" s="4">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I54" s="4">
         <v>0</v>
       </c>
       <c r="J54" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="K54" s="19" t="s">
-        <v>151</v>
+        <v>127</v>
       </c>
       <c r="M54" s="19" t="s">
-        <v>182</v>
+        <v>158</v>
       </c>
       <c r="N54" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>Complete</v>
+        <v>In Progress</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>